<commit_message>
Committing new Excel file with data.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owner/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owner/Desktop/Distributed Computing/Projects/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -175,10 +175,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data!$C$2:$C$111</c:f>
+              <c:f>data!$C$2:$C$346</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="110"/>
+                <c:ptCount val="345"/>
                 <c:pt idx="0">
                   <c:v>1338.0</c:v>
                 </c:pt>
@@ -508,6 +508,711 @@
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1037.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1020.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1021.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1021.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1017.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1020.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1016.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1014.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1072.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1063.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1016.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1019.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1045.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1020.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1034.0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1094.0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1226.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1162.0</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1014.0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1023.0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1016.0</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1074.0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1023.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1036.0</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1028.0</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1034.0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1018.0</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1019.0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>1054.0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1073.0</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1076.0</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1137.0</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1018.0</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1060.0</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1029.0</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1019.0</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1053.0</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>1018.0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1022.0</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1066.0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1018.0</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1005.0</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1179.0</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1033.0</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1017.0</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1106.0</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1004.0</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1014.0</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1018.0</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1077.0</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1014.0</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1856.0</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1005.0</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1021.0</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>1817.0</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>1003.0</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>1019.0</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>1023.0</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>1018.0</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>1022.0</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>1141.0</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>1256.0</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>1012.0</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>1033.0</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>1002.0</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>1014.0</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>1061.0</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>1006.0</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>1021.0</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1016.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>1077.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>1007.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>1013.0</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>1009.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,11 +1228,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2025838112"/>
-        <c:axId val="-2025835552"/>
+        <c:axId val="-2103130624"/>
+        <c:axId val="-2049079792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2025838112"/>
+        <c:axId val="-2103130624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,7 +1273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2025835552"/>
+        <c:crossAx val="-2049079792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +1281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2025835552"/>
+        <c:axId val="-2049079792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +1331,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2025838112"/>
+        <c:crossAx val="-2103130624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -813,6 +1518,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Transmission In Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
@@ -833,10 +1549,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data!$B$2:$B$111</c:f>
+              <c:f>data!$B$2:$B$346</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="110"/>
+                <c:ptCount val="345"/>
                 <c:pt idx="0">
                   <c:v>549.0</c:v>
                 </c:pt>
@@ -1165,6 +1881,711 @@
                   <c:v>549.0</c:v>
                 </c:pt>
                 <c:pt idx="109">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>549.0</c:v>
+                </c:pt>
+                <c:pt idx="344">
                   <c:v>549.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1181,11 +2602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2027480240"/>
-        <c:axId val="-2025528672"/>
+        <c:axId val="-2035732096"/>
+        <c:axId val="-2035779664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2027480240"/>
+        <c:axId val="-2035732096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,7 +2647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2025528672"/>
+        <c:crossAx val="-2035779664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1234,7 +2655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2025528672"/>
+        <c:axId val="-2035779664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +2705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2027480240"/>
+        <c:crossAx val="-2035732096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1446,6 +2867,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Transmission Out Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
@@ -1466,10 +2898,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data!$A$2:$A$111</c:f>
+              <c:f>data!$A$2:$A$346</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="110"/>
+                <c:ptCount val="345"/>
                 <c:pt idx="0">
                   <c:v>500.0</c:v>
                 </c:pt>
@@ -1798,6 +3230,711 @@
                   <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="109">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="344">
                   <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1814,11 +3951,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2051386016"/>
-        <c:axId val="-2021152352"/>
+        <c:axId val="-2035694624"/>
+        <c:axId val="-2030910272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2051386016"/>
+        <c:axId val="-2035694624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +3996,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2021152352"/>
+        <c:crossAx val="-2030910272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1867,7 +4004,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021152352"/>
+        <c:axId val="-2030910272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1917,7 +4054,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051386016"/>
+        <c:crossAx val="-2035694624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3943,16 +6080,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C346"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5173,6 +7307,2591 @@
       </c>
       <c r="C111">
         <v>1011</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>500</v>
+      </c>
+      <c r="B112">
+        <v>549</v>
+      </c>
+      <c r="C112">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>500</v>
+      </c>
+      <c r="B113">
+        <v>549</v>
+      </c>
+      <c r="C113">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>500</v>
+      </c>
+      <c r="B114">
+        <v>549</v>
+      </c>
+      <c r="C114">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>500</v>
+      </c>
+      <c r="B115">
+        <v>549</v>
+      </c>
+      <c r="C115">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>500</v>
+      </c>
+      <c r="B116">
+        <v>549</v>
+      </c>
+      <c r="C116">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>500</v>
+      </c>
+      <c r="B117">
+        <v>549</v>
+      </c>
+      <c r="C117">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>500</v>
+      </c>
+      <c r="B118">
+        <v>549</v>
+      </c>
+      <c r="C118">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>500</v>
+      </c>
+      <c r="B119">
+        <v>549</v>
+      </c>
+      <c r="C119">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>500</v>
+      </c>
+      <c r="B120">
+        <v>549</v>
+      </c>
+      <c r="C120">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>500</v>
+      </c>
+      <c r="B121">
+        <v>549</v>
+      </c>
+      <c r="C121">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>500</v>
+      </c>
+      <c r="B122">
+        <v>549</v>
+      </c>
+      <c r="C122">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>500</v>
+      </c>
+      <c r="B123">
+        <v>549</v>
+      </c>
+      <c r="C123">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>500</v>
+      </c>
+      <c r="B124">
+        <v>549</v>
+      </c>
+      <c r="C124">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>500</v>
+      </c>
+      <c r="B125">
+        <v>549</v>
+      </c>
+      <c r="C125">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>500</v>
+      </c>
+      <c r="B126">
+        <v>549</v>
+      </c>
+      <c r="C126">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>500</v>
+      </c>
+      <c r="B127">
+        <v>549</v>
+      </c>
+      <c r="C127">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>500</v>
+      </c>
+      <c r="B128">
+        <v>549</v>
+      </c>
+      <c r="C128">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>500</v>
+      </c>
+      <c r="B129">
+        <v>549</v>
+      </c>
+      <c r="C129">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>500</v>
+      </c>
+      <c r="B130">
+        <v>549</v>
+      </c>
+      <c r="C130">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>500</v>
+      </c>
+      <c r="B131">
+        <v>549</v>
+      </c>
+      <c r="C131">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>500</v>
+      </c>
+      <c r="B132">
+        <v>549</v>
+      </c>
+      <c r="C132">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>500</v>
+      </c>
+      <c r="B133">
+        <v>549</v>
+      </c>
+      <c r="C133">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>500</v>
+      </c>
+      <c r="B134">
+        <v>549</v>
+      </c>
+      <c r="C134">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>500</v>
+      </c>
+      <c r="B135">
+        <v>549</v>
+      </c>
+      <c r="C135">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>500</v>
+      </c>
+      <c r="B136">
+        <v>549</v>
+      </c>
+      <c r="C136">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>500</v>
+      </c>
+      <c r="B137">
+        <v>549</v>
+      </c>
+      <c r="C137">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>500</v>
+      </c>
+      <c r="B138">
+        <v>549</v>
+      </c>
+      <c r="C138">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>500</v>
+      </c>
+      <c r="B139">
+        <v>549</v>
+      </c>
+      <c r="C139">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>500</v>
+      </c>
+      <c r="B140">
+        <v>549</v>
+      </c>
+      <c r="C140">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>500</v>
+      </c>
+      <c r="B141">
+        <v>549</v>
+      </c>
+      <c r="C141">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>500</v>
+      </c>
+      <c r="B142">
+        <v>549</v>
+      </c>
+      <c r="C142">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>500</v>
+      </c>
+      <c r="B143">
+        <v>549</v>
+      </c>
+      <c r="C143">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>500</v>
+      </c>
+      <c r="B144">
+        <v>549</v>
+      </c>
+      <c r="C144">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>500</v>
+      </c>
+      <c r="B145">
+        <v>549</v>
+      </c>
+      <c r="C145">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>500</v>
+      </c>
+      <c r="B146">
+        <v>549</v>
+      </c>
+      <c r="C146">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>500</v>
+      </c>
+      <c r="B147">
+        <v>549</v>
+      </c>
+      <c r="C147">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>500</v>
+      </c>
+      <c r="B148">
+        <v>549</v>
+      </c>
+      <c r="C148">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>500</v>
+      </c>
+      <c r="B149">
+        <v>549</v>
+      </c>
+      <c r="C149">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>500</v>
+      </c>
+      <c r="B150">
+        <v>549</v>
+      </c>
+      <c r="C150">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>500</v>
+      </c>
+      <c r="B151">
+        <v>549</v>
+      </c>
+      <c r="C151">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>500</v>
+      </c>
+      <c r="B152">
+        <v>549</v>
+      </c>
+      <c r="C152">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>500</v>
+      </c>
+      <c r="B153">
+        <v>549</v>
+      </c>
+      <c r="C153">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>500</v>
+      </c>
+      <c r="B154">
+        <v>549</v>
+      </c>
+      <c r="C154">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>500</v>
+      </c>
+      <c r="B155">
+        <v>549</v>
+      </c>
+      <c r="C155">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>500</v>
+      </c>
+      <c r="B156">
+        <v>549</v>
+      </c>
+      <c r="C156">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>500</v>
+      </c>
+      <c r="B157">
+        <v>549</v>
+      </c>
+      <c r="C157">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>500</v>
+      </c>
+      <c r="B158">
+        <v>549</v>
+      </c>
+      <c r="C158">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>500</v>
+      </c>
+      <c r="B159">
+        <v>549</v>
+      </c>
+      <c r="C159">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>500</v>
+      </c>
+      <c r="B160">
+        <v>549</v>
+      </c>
+      <c r="C160">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>500</v>
+      </c>
+      <c r="B161">
+        <v>549</v>
+      </c>
+      <c r="C161">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>500</v>
+      </c>
+      <c r="B162">
+        <v>549</v>
+      </c>
+      <c r="C162">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>500</v>
+      </c>
+      <c r="B163">
+        <v>549</v>
+      </c>
+      <c r="C163">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>500</v>
+      </c>
+      <c r="B164">
+        <v>549</v>
+      </c>
+      <c r="C164">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>500</v>
+      </c>
+      <c r="B165">
+        <v>549</v>
+      </c>
+      <c r="C165">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>500</v>
+      </c>
+      <c r="B166">
+        <v>549</v>
+      </c>
+      <c r="C166">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>500</v>
+      </c>
+      <c r="B167">
+        <v>549</v>
+      </c>
+      <c r="C167">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>500</v>
+      </c>
+      <c r="B168">
+        <v>549</v>
+      </c>
+      <c r="C168">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>500</v>
+      </c>
+      <c r="B169">
+        <v>549</v>
+      </c>
+      <c r="C169">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>500</v>
+      </c>
+      <c r="B170">
+        <v>549</v>
+      </c>
+      <c r="C170">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>500</v>
+      </c>
+      <c r="B171">
+        <v>549</v>
+      </c>
+      <c r="C171">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>500</v>
+      </c>
+      <c r="B172">
+        <v>549</v>
+      </c>
+      <c r="C172">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>500</v>
+      </c>
+      <c r="B173">
+        <v>549</v>
+      </c>
+      <c r="C173">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>500</v>
+      </c>
+      <c r="B174">
+        <v>549</v>
+      </c>
+      <c r="C174">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>500</v>
+      </c>
+      <c r="B175">
+        <v>549</v>
+      </c>
+      <c r="C175">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>500</v>
+      </c>
+      <c r="B176">
+        <v>549</v>
+      </c>
+      <c r="C176">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>500</v>
+      </c>
+      <c r="B177">
+        <v>549</v>
+      </c>
+      <c r="C177">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>500</v>
+      </c>
+      <c r="B178">
+        <v>549</v>
+      </c>
+      <c r="C178">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>500</v>
+      </c>
+      <c r="B179">
+        <v>549</v>
+      </c>
+      <c r="C179">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>500</v>
+      </c>
+      <c r="B180">
+        <v>549</v>
+      </c>
+      <c r="C180">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>500</v>
+      </c>
+      <c r="B181">
+        <v>549</v>
+      </c>
+      <c r="C181">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>500</v>
+      </c>
+      <c r="B182">
+        <v>549</v>
+      </c>
+      <c r="C182">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>500</v>
+      </c>
+      <c r="B183">
+        <v>549</v>
+      </c>
+      <c r="C183">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>500</v>
+      </c>
+      <c r="B184">
+        <v>549</v>
+      </c>
+      <c r="C184">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>500</v>
+      </c>
+      <c r="B185">
+        <v>549</v>
+      </c>
+      <c r="C185">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>500</v>
+      </c>
+      <c r="B186">
+        <v>549</v>
+      </c>
+      <c r="C186">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>500</v>
+      </c>
+      <c r="B187">
+        <v>549</v>
+      </c>
+      <c r="C187">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>500</v>
+      </c>
+      <c r="B188">
+        <v>549</v>
+      </c>
+      <c r="C188">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>500</v>
+      </c>
+      <c r="B189">
+        <v>549</v>
+      </c>
+      <c r="C189">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>500</v>
+      </c>
+      <c r="B190">
+        <v>549</v>
+      </c>
+      <c r="C190">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>500</v>
+      </c>
+      <c r="B191">
+        <v>549</v>
+      </c>
+      <c r="C191">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>500</v>
+      </c>
+      <c r="B192">
+        <v>549</v>
+      </c>
+      <c r="C192">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>500</v>
+      </c>
+      <c r="B193">
+        <v>549</v>
+      </c>
+      <c r="C193">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>500</v>
+      </c>
+      <c r="B194">
+        <v>549</v>
+      </c>
+      <c r="C194">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>500</v>
+      </c>
+      <c r="B195">
+        <v>549</v>
+      </c>
+      <c r="C195">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>500</v>
+      </c>
+      <c r="B196">
+        <v>549</v>
+      </c>
+      <c r="C196">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>500</v>
+      </c>
+      <c r="B197">
+        <v>549</v>
+      </c>
+      <c r="C197">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>500</v>
+      </c>
+      <c r="B198">
+        <v>549</v>
+      </c>
+      <c r="C198">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>500</v>
+      </c>
+      <c r="B199">
+        <v>549</v>
+      </c>
+      <c r="C199">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>500</v>
+      </c>
+      <c r="B200">
+        <v>549</v>
+      </c>
+      <c r="C200">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>500</v>
+      </c>
+      <c r="B201">
+        <v>549</v>
+      </c>
+      <c r="C201">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>500</v>
+      </c>
+      <c r="B202">
+        <v>549</v>
+      </c>
+      <c r="C202">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>500</v>
+      </c>
+      <c r="B203">
+        <v>549</v>
+      </c>
+      <c r="C203">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>500</v>
+      </c>
+      <c r="B204">
+        <v>549</v>
+      </c>
+      <c r="C204">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>500</v>
+      </c>
+      <c r="B205">
+        <v>549</v>
+      </c>
+      <c r="C205">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>500</v>
+      </c>
+      <c r="B206">
+        <v>549</v>
+      </c>
+      <c r="C206">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>500</v>
+      </c>
+      <c r="B207">
+        <v>549</v>
+      </c>
+      <c r="C207">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>500</v>
+      </c>
+      <c r="B208">
+        <v>549</v>
+      </c>
+      <c r="C208">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>500</v>
+      </c>
+      <c r="B209">
+        <v>549</v>
+      </c>
+      <c r="C209">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>500</v>
+      </c>
+      <c r="B210">
+        <v>549</v>
+      </c>
+      <c r="C210">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>500</v>
+      </c>
+      <c r="B211">
+        <v>549</v>
+      </c>
+      <c r="C211">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>500</v>
+      </c>
+      <c r="B212">
+        <v>549</v>
+      </c>
+      <c r="C212">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>500</v>
+      </c>
+      <c r="B213">
+        <v>549</v>
+      </c>
+      <c r="C213">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>500</v>
+      </c>
+      <c r="B214">
+        <v>549</v>
+      </c>
+      <c r="C214">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>500</v>
+      </c>
+      <c r="B215">
+        <v>549</v>
+      </c>
+      <c r="C215">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>500</v>
+      </c>
+      <c r="B216">
+        <v>549</v>
+      </c>
+      <c r="C216">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>500</v>
+      </c>
+      <c r="B217">
+        <v>549</v>
+      </c>
+      <c r="C217">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>500</v>
+      </c>
+      <c r="B218">
+        <v>549</v>
+      </c>
+      <c r="C218">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>500</v>
+      </c>
+      <c r="B219">
+        <v>549</v>
+      </c>
+      <c r="C219">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>500</v>
+      </c>
+      <c r="B220">
+        <v>549</v>
+      </c>
+      <c r="C220">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>500</v>
+      </c>
+      <c r="B221">
+        <v>549</v>
+      </c>
+      <c r="C221">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>500</v>
+      </c>
+      <c r="B222">
+        <v>549</v>
+      </c>
+      <c r="C222">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>500</v>
+      </c>
+      <c r="B223">
+        <v>549</v>
+      </c>
+      <c r="C223">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>500</v>
+      </c>
+      <c r="B224">
+        <v>549</v>
+      </c>
+      <c r="C224">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>500</v>
+      </c>
+      <c r="B225">
+        <v>549</v>
+      </c>
+      <c r="C225">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>500</v>
+      </c>
+      <c r="B226">
+        <v>549</v>
+      </c>
+      <c r="C226">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>500</v>
+      </c>
+      <c r="B227">
+        <v>549</v>
+      </c>
+      <c r="C227">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>500</v>
+      </c>
+      <c r="B228">
+        <v>549</v>
+      </c>
+      <c r="C228">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>500</v>
+      </c>
+      <c r="B229">
+        <v>549</v>
+      </c>
+      <c r="C229">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>500</v>
+      </c>
+      <c r="B230">
+        <v>549</v>
+      </c>
+      <c r="C230">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>500</v>
+      </c>
+      <c r="B231">
+        <v>549</v>
+      </c>
+      <c r="C231">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>500</v>
+      </c>
+      <c r="B232">
+        <v>549</v>
+      </c>
+      <c r="C232">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>500</v>
+      </c>
+      <c r="B233">
+        <v>549</v>
+      </c>
+      <c r="C233">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>500</v>
+      </c>
+      <c r="B234">
+        <v>549</v>
+      </c>
+      <c r="C234">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>500</v>
+      </c>
+      <c r="B235">
+        <v>549</v>
+      </c>
+      <c r="C235">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>500</v>
+      </c>
+      <c r="B236">
+        <v>549</v>
+      </c>
+      <c r="C236">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>500</v>
+      </c>
+      <c r="B237">
+        <v>549</v>
+      </c>
+      <c r="C237">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>500</v>
+      </c>
+      <c r="B238">
+        <v>549</v>
+      </c>
+      <c r="C238">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>500</v>
+      </c>
+      <c r="B239">
+        <v>549</v>
+      </c>
+      <c r="C239">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>500</v>
+      </c>
+      <c r="B240">
+        <v>549</v>
+      </c>
+      <c r="C240">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>500</v>
+      </c>
+      <c r="B241">
+        <v>549</v>
+      </c>
+      <c r="C241">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>500</v>
+      </c>
+      <c r="B242">
+        <v>549</v>
+      </c>
+      <c r="C242">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>500</v>
+      </c>
+      <c r="B243">
+        <v>549</v>
+      </c>
+      <c r="C243">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>500</v>
+      </c>
+      <c r="B244">
+        <v>549</v>
+      </c>
+      <c r="C244">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>500</v>
+      </c>
+      <c r="B245">
+        <v>549</v>
+      </c>
+      <c r="C245">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>500</v>
+      </c>
+      <c r="B246">
+        <v>549</v>
+      </c>
+      <c r="C246">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>500</v>
+      </c>
+      <c r="B247">
+        <v>549</v>
+      </c>
+      <c r="C247">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>500</v>
+      </c>
+      <c r="B248">
+        <v>549</v>
+      </c>
+      <c r="C248">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>500</v>
+      </c>
+      <c r="B249">
+        <v>549</v>
+      </c>
+      <c r="C249">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>500</v>
+      </c>
+      <c r="B250">
+        <v>549</v>
+      </c>
+      <c r="C250">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>500</v>
+      </c>
+      <c r="B251">
+        <v>549</v>
+      </c>
+      <c r="C251">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>500</v>
+      </c>
+      <c r="B252">
+        <v>549</v>
+      </c>
+      <c r="C252">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>500</v>
+      </c>
+      <c r="B253">
+        <v>549</v>
+      </c>
+      <c r="C253">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>500</v>
+      </c>
+      <c r="B254">
+        <v>549</v>
+      </c>
+      <c r="C254">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>500</v>
+      </c>
+      <c r="B255">
+        <v>549</v>
+      </c>
+      <c r="C255">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>500</v>
+      </c>
+      <c r="B256">
+        <v>549</v>
+      </c>
+      <c r="C256">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>500</v>
+      </c>
+      <c r="B257">
+        <v>549</v>
+      </c>
+      <c r="C257">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>500</v>
+      </c>
+      <c r="B258">
+        <v>549</v>
+      </c>
+      <c r="C258">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>500</v>
+      </c>
+      <c r="B259">
+        <v>549</v>
+      </c>
+      <c r="C259">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>500</v>
+      </c>
+      <c r="B260">
+        <v>549</v>
+      </c>
+      <c r="C260">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>500</v>
+      </c>
+      <c r="B261">
+        <v>549</v>
+      </c>
+      <c r="C261">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>500</v>
+      </c>
+      <c r="B262">
+        <v>549</v>
+      </c>
+      <c r="C262">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>500</v>
+      </c>
+      <c r="B263">
+        <v>549</v>
+      </c>
+      <c r="C263">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>500</v>
+      </c>
+      <c r="B264">
+        <v>549</v>
+      </c>
+      <c r="C264">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>500</v>
+      </c>
+      <c r="B265">
+        <v>549</v>
+      </c>
+      <c r="C265">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>500</v>
+      </c>
+      <c r="B266">
+        <v>549</v>
+      </c>
+      <c r="C266">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>500</v>
+      </c>
+      <c r="B267">
+        <v>549</v>
+      </c>
+      <c r="C267">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>500</v>
+      </c>
+      <c r="B268">
+        <v>549</v>
+      </c>
+      <c r="C268">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>500</v>
+      </c>
+      <c r="B269">
+        <v>549</v>
+      </c>
+      <c r="C269">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>500</v>
+      </c>
+      <c r="B270">
+        <v>549</v>
+      </c>
+      <c r="C270">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>500</v>
+      </c>
+      <c r="B271">
+        <v>549</v>
+      </c>
+      <c r="C271">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>500</v>
+      </c>
+      <c r="B272">
+        <v>549</v>
+      </c>
+      <c r="C272">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>500</v>
+      </c>
+      <c r="B273">
+        <v>549</v>
+      </c>
+      <c r="C273">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>500</v>
+      </c>
+      <c r="B274">
+        <v>549</v>
+      </c>
+      <c r="C274">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>500</v>
+      </c>
+      <c r="B275">
+        <v>549</v>
+      </c>
+      <c r="C275">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>500</v>
+      </c>
+      <c r="B276">
+        <v>549</v>
+      </c>
+      <c r="C276">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>500</v>
+      </c>
+      <c r="B277">
+        <v>549</v>
+      </c>
+      <c r="C277">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>500</v>
+      </c>
+      <c r="B278">
+        <v>549</v>
+      </c>
+      <c r="C278">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>500</v>
+      </c>
+      <c r="B279">
+        <v>549</v>
+      </c>
+      <c r="C279">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>500</v>
+      </c>
+      <c r="B280">
+        <v>549</v>
+      </c>
+      <c r="C280">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>500</v>
+      </c>
+      <c r="B281">
+        <v>549</v>
+      </c>
+      <c r="C281">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>500</v>
+      </c>
+      <c r="B282">
+        <v>549</v>
+      </c>
+      <c r="C282">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>500</v>
+      </c>
+      <c r="B283">
+        <v>549</v>
+      </c>
+      <c r="C283">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>500</v>
+      </c>
+      <c r="B284">
+        <v>549</v>
+      </c>
+      <c r="C284">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>500</v>
+      </c>
+      <c r="B285">
+        <v>549</v>
+      </c>
+      <c r="C285">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>500</v>
+      </c>
+      <c r="B286">
+        <v>549</v>
+      </c>
+      <c r="C286">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>500</v>
+      </c>
+      <c r="B287">
+        <v>549</v>
+      </c>
+      <c r="C287">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>500</v>
+      </c>
+      <c r="B288">
+        <v>549</v>
+      </c>
+      <c r="C288">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>500</v>
+      </c>
+      <c r="B289">
+        <v>549</v>
+      </c>
+      <c r="C289">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>500</v>
+      </c>
+      <c r="B290">
+        <v>549</v>
+      </c>
+      <c r="C290">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>500</v>
+      </c>
+      <c r="B291">
+        <v>549</v>
+      </c>
+      <c r="C291">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>500</v>
+      </c>
+      <c r="B292">
+        <v>549</v>
+      </c>
+      <c r="C292">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>500</v>
+      </c>
+      <c r="B293">
+        <v>549</v>
+      </c>
+      <c r="C293">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>500</v>
+      </c>
+      <c r="B294">
+        <v>549</v>
+      </c>
+      <c r="C294">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>500</v>
+      </c>
+      <c r="B295">
+        <v>549</v>
+      </c>
+      <c r="C295">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>500</v>
+      </c>
+      <c r="B296">
+        <v>549</v>
+      </c>
+      <c r="C296">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>500</v>
+      </c>
+      <c r="B297">
+        <v>549</v>
+      </c>
+      <c r="C297">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>500</v>
+      </c>
+      <c r="B298">
+        <v>549</v>
+      </c>
+      <c r="C298">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>500</v>
+      </c>
+      <c r="B299">
+        <v>549</v>
+      </c>
+      <c r="C299">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>500</v>
+      </c>
+      <c r="B300">
+        <v>549</v>
+      </c>
+      <c r="C300">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>500</v>
+      </c>
+      <c r="B301">
+        <v>549</v>
+      </c>
+      <c r="C301">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>500</v>
+      </c>
+      <c r="B302">
+        <v>549</v>
+      </c>
+      <c r="C302">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>500</v>
+      </c>
+      <c r="B303">
+        <v>549</v>
+      </c>
+      <c r="C303">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>500</v>
+      </c>
+      <c r="B304">
+        <v>549</v>
+      </c>
+      <c r="C304">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>500</v>
+      </c>
+      <c r="B305">
+        <v>549</v>
+      </c>
+      <c r="C305">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>500</v>
+      </c>
+      <c r="B306">
+        <v>549</v>
+      </c>
+      <c r="C306">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>500</v>
+      </c>
+      <c r="B307">
+        <v>549</v>
+      </c>
+      <c r="C307">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>500</v>
+      </c>
+      <c r="B308">
+        <v>549</v>
+      </c>
+      <c r="C308">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>500</v>
+      </c>
+      <c r="B309">
+        <v>549</v>
+      </c>
+      <c r="C309">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>500</v>
+      </c>
+      <c r="B310">
+        <v>549</v>
+      </c>
+      <c r="C310">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>500</v>
+      </c>
+      <c r="B311">
+        <v>549</v>
+      </c>
+      <c r="C311">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>500</v>
+      </c>
+      <c r="B312">
+        <v>549</v>
+      </c>
+      <c r="C312">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>500</v>
+      </c>
+      <c r="B313">
+        <v>549</v>
+      </c>
+      <c r="C313">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>500</v>
+      </c>
+      <c r="B314">
+        <v>549</v>
+      </c>
+      <c r="C314">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>500</v>
+      </c>
+      <c r="B315">
+        <v>549</v>
+      </c>
+      <c r="C315">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>500</v>
+      </c>
+      <c r="B316">
+        <v>549</v>
+      </c>
+      <c r="C316">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>500</v>
+      </c>
+      <c r="B317">
+        <v>549</v>
+      </c>
+      <c r="C317">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>500</v>
+      </c>
+      <c r="B318">
+        <v>549</v>
+      </c>
+      <c r="C318">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>500</v>
+      </c>
+      <c r="B319">
+        <v>549</v>
+      </c>
+      <c r="C319">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>500</v>
+      </c>
+      <c r="B320">
+        <v>549</v>
+      </c>
+      <c r="C320">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>500</v>
+      </c>
+      <c r="B321">
+        <v>549</v>
+      </c>
+      <c r="C321">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>500</v>
+      </c>
+      <c r="B322">
+        <v>549</v>
+      </c>
+      <c r="C322">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>500</v>
+      </c>
+      <c r="B323">
+        <v>549</v>
+      </c>
+      <c r="C323">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>500</v>
+      </c>
+      <c r="B324">
+        <v>549</v>
+      </c>
+      <c r="C324">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>500</v>
+      </c>
+      <c r="B325">
+        <v>549</v>
+      </c>
+      <c r="C325">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>500</v>
+      </c>
+      <c r="B326">
+        <v>549</v>
+      </c>
+      <c r="C326">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>500</v>
+      </c>
+      <c r="B327">
+        <v>549</v>
+      </c>
+      <c r="C327">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <v>500</v>
+      </c>
+      <c r="B328">
+        <v>549</v>
+      </c>
+      <c r="C328">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <v>500</v>
+      </c>
+      <c r="B329">
+        <v>549</v>
+      </c>
+      <c r="C329">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>500</v>
+      </c>
+      <c r="B330">
+        <v>549</v>
+      </c>
+      <c r="C330">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>500</v>
+      </c>
+      <c r="B331">
+        <v>549</v>
+      </c>
+      <c r="C331">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>500</v>
+      </c>
+      <c r="B332">
+        <v>549</v>
+      </c>
+      <c r="C332">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>500</v>
+      </c>
+      <c r="B333">
+        <v>549</v>
+      </c>
+      <c r="C333">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>500</v>
+      </c>
+      <c r="B334">
+        <v>549</v>
+      </c>
+      <c r="C334">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <v>500</v>
+      </c>
+      <c r="B335">
+        <v>549</v>
+      </c>
+      <c r="C335">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <v>500</v>
+      </c>
+      <c r="B336">
+        <v>549</v>
+      </c>
+      <c r="C336">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <v>500</v>
+      </c>
+      <c r="B337">
+        <v>549</v>
+      </c>
+      <c r="C337">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>500</v>
+      </c>
+      <c r="B338">
+        <v>549</v>
+      </c>
+      <c r="C338">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A339">
+        <v>500</v>
+      </c>
+      <c r="B339">
+        <v>549</v>
+      </c>
+      <c r="C339">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <v>500</v>
+      </c>
+      <c r="B340">
+        <v>549</v>
+      </c>
+      <c r="C340">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <v>500</v>
+      </c>
+      <c r="B341">
+        <v>549</v>
+      </c>
+      <c r="C341">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <v>500</v>
+      </c>
+      <c r="B342">
+        <v>549</v>
+      </c>
+      <c r="C342">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <v>500</v>
+      </c>
+      <c r="B343">
+        <v>549</v>
+      </c>
+      <c r="C343">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <v>500</v>
+      </c>
+      <c r="B344">
+        <v>549</v>
+      </c>
+      <c r="C344">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <v>500</v>
+      </c>
+      <c r="B345">
+        <v>549</v>
+      </c>
+      <c r="C345">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <v>500</v>
+      </c>
+      <c r="B346">
+        <v>549</v>
+      </c>
+      <c r="C346">
+        <v>1009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>